<commit_message>
agency fiscal year downloaded data files
</commit_message>
<xml_diff>
--- a/AnnualSRSSummaryReport/ReturnA/ByAgency/FiscalYearData/SRS_AnnualSummary_ReturnA (1).xlsx
+++ b/AnnualSRSSummaryReport/ReturnA/ByAgency/FiscalYearData/SRS_AnnualSummary_ReturnA (1).xlsx
@@ -376,7 +376,7 @@
     <row r="3" ht="7.5" customHeight="1">
       <c s="1" t="inlineStr" r="M3">
         <is>
-          <t xml:space="preserve">Printed On: 10/22/2025</t>
+          <t xml:space="preserve">Printed On: 10/23/2025</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
               <color rgb="FF000000"/>
               <rFont val="verdana"/>
             </rPr>
-            <t xml:space="preserve"> GETTYSBURG BOROUGH</t>
+            <t xml:space="preserve"> LITTLESTOWN BOROUGH</t>
           </r>
         </is>
       </c>
@@ -838,7 +838,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">4</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -872,7 +872,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">4</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -888,7 +888,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -944,7 +944,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -978,7 +978,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -1050,7 +1050,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -1084,7 +1084,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -1100,7 +1100,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -1156,7 +1156,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">1</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -1190,7 +1190,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">1</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -1262,7 +1262,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">1</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -1296,7 +1296,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">1</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -1686,7 +1686,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">9</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -1720,7 +1720,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">9</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -1736,7 +1736,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">4</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -1792,7 +1792,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">0</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -1826,7 +1826,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">0</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -1898,7 +1898,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -1932,7 +1932,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -1948,7 +1948,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -2004,7 +2004,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -2038,7 +2038,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -2054,7 +2054,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">1</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -2110,7 +2110,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">5</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -2144,7 +2144,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">5</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -2160,7 +2160,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">1</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -2216,7 +2216,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">6</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -2250,7 +2250,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">6</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -2266,7 +2266,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">3</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -2428,7 +2428,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">6</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -2462,7 +2462,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">6</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -2478,7 +2478,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">3</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -2690,7 +2690,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">26</t>
+            <t xml:space="preserve">22</t>
           </r>
         </is>
       </c>
@@ -2709,7 +2709,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">3</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -3170,7 +3170,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">1</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -3204,7 +3204,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">1</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -3220,7 +3220,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">1</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -3382,7 +3382,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">51</t>
+            <t xml:space="preserve">33</t>
           </r>
         </is>
       </c>
@@ -3416,7 +3416,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">51</t>
+            <t xml:space="preserve">33</t>
           </r>
         </is>
       </c>
@@ -3432,7 +3432,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">36</t>
+            <t xml:space="preserve">24</t>
           </r>
         </is>
       </c>
@@ -3451,7 +3451,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">3</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -3488,7 +3488,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">86</t>
+            <t xml:space="preserve">9</t>
           </r>
         </is>
       </c>
@@ -3522,7 +3522,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">86</t>
+            <t xml:space="preserve">9</t>
           </r>
         </is>
       </c>
@@ -3538,7 +3538,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">72</t>
+            <t xml:space="preserve">12</t>
           </r>
         </is>
       </c>
@@ -3557,7 +3557,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">5</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -3594,7 +3594,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">5</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -3628,7 +3628,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">5</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -3644,7 +3644,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">6</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -3700,7 +3700,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">30</t>
+            <t xml:space="preserve">5</t>
           </r>
         </is>
       </c>
@@ -3734,7 +3734,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">30</t>
+            <t xml:space="preserve">5</t>
           </r>
         </is>
       </c>
@@ -3750,7 +3750,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">29</t>
+            <t xml:space="preserve">5</t>
           </r>
         </is>
       </c>
@@ -3769,7 +3769,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">3</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -3806,7 +3806,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -3840,7 +3840,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -3856,7 +3856,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -3912,7 +3912,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">3</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -3946,7 +3946,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">3</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -3981,7 +3981,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">0</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -4018,7 +4018,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">25</t>
+            <t xml:space="preserve">6</t>
           </r>
         </is>
       </c>
@@ -4052,7 +4052,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">25</t>
+            <t xml:space="preserve">6</t>
           </r>
         </is>
       </c>
@@ -4068,7 +4068,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">11</t>
+            <t xml:space="preserve">6</t>
           </r>
         </is>
       </c>
@@ -4087,7 +4087,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">0</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -4124,7 +4124,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">5</t>
           </r>
         </is>
       </c>
@@ -4158,23 +4158,23 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
+            <t xml:space="preserve">5</t>
+          </r>
+        </is>
+      </c>
+      <c s="16" t="inlineStr" r="J52">
+        <is>
+          <r>
+            <rPr>
+              <b val="0"/>
+              <i val="0"/>
+              <strike val="0"/>
+              <u val="none"/>
+              <sz val="9"/>
+              <color rgb="FF000000"/>
+              <rFont val="Arial"/>
+            </rPr>
             <t xml:space="preserve">2</t>
-          </r>
-        </is>
-      </c>
-      <c s="16" t="inlineStr" r="J52">
-        <is>
-          <r>
-            <rPr>
-              <b val="0"/>
-              <i val="0"/>
-              <strike val="0"/>
-              <u val="none"/>
-              <sz val="9"/>
-              <color rgb="FF000000"/>
-              <rFont val="Arial"/>
-            </rPr>
-            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -4336,7 +4336,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">4</t>
+            <t xml:space="preserve">3</t>
           </r>
         </is>
       </c>
@@ -4370,7 +4370,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">4</t>
+            <t xml:space="preserve">3</t>
           </r>
         </is>
       </c>
@@ -4386,7 +4386,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">8</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -4405,7 +4405,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -4442,7 +4442,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">50</t>
+            <t xml:space="preserve">24</t>
           </r>
         </is>
       </c>
@@ -4476,7 +4476,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">50</t>
+            <t xml:space="preserve">24</t>
           </r>
         </is>
       </c>
@@ -4492,7 +4492,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">37</t>
+            <t xml:space="preserve">26</t>
           </r>
         </is>
       </c>
@@ -5078,7 +5078,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">50</t>
+            <t xml:space="preserve">24</t>
           </r>
         </is>
       </c>
@@ -5112,7 +5112,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">50</t>
+            <t xml:space="preserve">24</t>
           </r>
         </is>
       </c>
@@ -5128,7 +5128,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">37</t>
+            <t xml:space="preserve">26</t>
           </r>
         </is>
       </c>
@@ -5184,7 +5184,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -5218,7 +5218,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -5290,7 +5290,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">36</t>
+            <t xml:space="preserve">20</t>
           </r>
         </is>
       </c>
@@ -5324,7 +5324,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">36</t>
+            <t xml:space="preserve">20</t>
           </r>
         </is>
       </c>
@@ -5340,7 +5340,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">29</t>
+            <t xml:space="preserve">22</t>
           </r>
         </is>
       </c>
@@ -5396,7 +5396,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">0</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -5430,7 +5430,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">0</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -5446,7 +5446,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">0</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -5502,7 +5502,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">12</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -5536,7 +5536,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">12</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -5552,7 +5552,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">7</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -6138,7 +6138,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">175</t>
+            <t xml:space="preserve">13</t>
           </r>
         </is>
       </c>
@@ -6172,7 +6172,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">175</t>
+            <t xml:space="preserve">13</t>
           </r>
         </is>
       </c>
@@ -6188,7 +6188,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">87</t>
+            <t xml:space="preserve">14</t>
           </r>
         </is>
       </c>
@@ -6244,7 +6244,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">25</t>
+            <t xml:space="preserve">3</t>
           </r>
         </is>
       </c>
@@ -6278,7 +6278,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">25</t>
+            <t xml:space="preserve">3</t>
           </r>
         </is>
       </c>
@@ -6294,7 +6294,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">18</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -6313,7 +6313,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">1</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -6350,7 +6350,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">24</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -6384,7 +6384,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">24</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -6400,7 +6400,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">20</t>
+            <t xml:space="preserve">1</t>
           </r>
         </is>
       </c>
@@ -6456,7 +6456,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">37</t>
+            <t xml:space="preserve">4</t>
           </r>
         </is>
       </c>
@@ -6490,7 +6490,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">37</t>
+            <t xml:space="preserve">4</t>
           </r>
         </is>
       </c>
@@ -6506,7 +6506,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">29</t>
+            <t xml:space="preserve">4</t>
           </r>
         </is>
       </c>
@@ -6668,7 +6668,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">63</t>
+            <t xml:space="preserve">14</t>
           </r>
         </is>
       </c>
@@ -6702,7 +6702,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">63</t>
+            <t xml:space="preserve">14</t>
           </r>
         </is>
       </c>
@@ -6718,7 +6718,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">48</t>
+            <t xml:space="preserve">13</t>
           </r>
         </is>
       </c>
@@ -6737,7 +6737,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">2</t>
+            <t xml:space="preserve">0</t>
           </r>
         </is>
       </c>
@@ -6774,7 +6774,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">531</t>
+            <t xml:space="preserve">90</t>
           </r>
         </is>
       </c>
@@ -6808,7 +6808,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">531</t>
+            <t xml:space="preserve">90</t>
           </r>
         </is>
       </c>
@@ -6824,7 +6824,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">370</t>
+            <t xml:space="preserve">88</t>
           </r>
         </is>
       </c>
@@ -6843,7 +6843,7 @@
               <color rgb="FF000000"/>
               <rFont val="Arial"/>
             </rPr>
-            <t xml:space="preserve">15</t>
+            <t xml:space="preserve">6</t>
           </r>
         </is>
       </c>

</xml_diff>